<commit_message>
Add translations to forms
</commit_message>
<xml_diff>
--- a/odkx/forms/fw_location.xlsx
+++ b/odkx/forms/fw_location.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="survey" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="model" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="table_specific_translations" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -49,97 +50,115 @@
     <t xml:space="preserve">required</t>
   </si>
   <si>
-    <t xml:space="preserve">display.prompt.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.hint.text</t>
+    <t xml:space="preserve">display.prompt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hint</t>
   </si>
   <si>
     <t xml:space="preserve">geopoint</t>
   </si>
   <si>
+    <t xml:space="preserve">hh_geo_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stand_outside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stand_outside.hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setting_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.title.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.title.text.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.title.text.sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.locale.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.locale.text.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.locale.text.sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">fw_location</t>
   </si>
   <si>
+    <t xml:space="preserve">form_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Worker Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Português</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiswahili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_row_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string_token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text.sw</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stand just outside the front door of the house and geocode the location.</t>
   </si>
   <si>
     <t xml:space="preserve">The household id is {{data.hh_id}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">setting_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.title.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.title.text.pt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.title.text.sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.locale.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.locale.text.pt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.locale.text.sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field Worker Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Português</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiswahili</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_row_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
   </si>
 </sst>
 </file>
@@ -244,6 +263,84 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Cascadia Mono SemiLight"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -254,11 +351,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -300,16 +397,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="74.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,26 +426,25 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -368,10 +465,10 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.03"/>
@@ -385,36 +482,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -422,7 +519,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210203001</v>
+        <v>20210204001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,7 +527,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +608,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
@@ -542,17 +639,17 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -565,4 +662,67 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.1328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:D1048576">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Add translations to forms"
This reverts commit d21aa63e051894407e7d2f4a3332b6900bd1b9a1.
</commit_message>
<xml_diff>
--- a/odkx/forms/fw_location.xlsx
+++ b/odkx/forms/fw_location.xlsx
@@ -5,14 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="survey" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="model" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="table_specific_translations" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -50,22 +49,25 @@
     <t xml:space="preserve">required</t>
   </si>
   <si>
-    <t xml:space="preserve">display.prompt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.hint</t>
+    <t xml:space="preserve">display.prompt.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hint.text</t>
   </si>
   <si>
     <t xml:space="preserve">geopoint</t>
   </si>
   <si>
-    <t xml:space="preserve">hh_geo_location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stand_outside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stand_outside.hint</t>
+    <t xml:space="preserve">fw_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand just outside the front door of the house and geocode the location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The household id is {{data.hh_id}}</t>
   </si>
   <si>
     <t xml:space="preserve">setting_name</t>
@@ -95,9 +97,6 @@
     <t xml:space="preserve">form_id</t>
   </si>
   <si>
-    <t xml:space="preserve">fw_location</t>
-  </si>
-  <si>
     <t xml:space="preserve">form_version</t>
   </si>
   <si>
@@ -141,24 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string_token</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text.pt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text.sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stand just outside the front door of the house and geocode the location.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The household id is {{data.hh_id}}</t>
   </si>
 </sst>
 </file>
@@ -263,84 +244,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <name val="Cascadia Mono SemiLight"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -351,11 +254,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -397,17 +300,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="74.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,25 +328,26 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -465,10 +368,10 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.03"/>
@@ -482,36 +385,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,7 +422,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210204001</v>
+        <v>20210203001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +430,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,7 +511,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
@@ -639,17 +542,17 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="0" t="s">
         <v>38</v>
       </c>
     </row>
@@ -662,67 +565,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.54"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B1:D1048576">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>